<commit_message>
2021-06-28 all snp files corrected, earlier attempt in 637dbeb was erroneous
</commit_message>
<xml_diff>
--- a/data/brain names and codes.xlsx
+++ b/data/brain names and codes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r0607671\Desktop\KUL-MPsy-Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdd34de6af154437/UU/Personal projects/KUL-MPsy-Thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="82" documentId="11_C71E6C79D2F240CBB0A60FE052DBA115DE8092C5" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F20683D2-7F68-4127-9536-CAF4CE9C19F9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="26190"/>
+    <workbookView xWindow="11890" yWindow="8330" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="brain names" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="166">
   <si>
     <t xml:space="preserve"> Sam Evrard</t>
   </si>
@@ -349,13 +350,181 @@
   </si>
   <si>
     <t>UC10</t>
+  </si>
+  <si>
+    <t>HC1</t>
+  </si>
+  <si>
+    <t>HC2</t>
+  </si>
+  <si>
+    <t>HC3</t>
+  </si>
+  <si>
+    <t>HC4</t>
+  </si>
+  <si>
+    <t>HC5</t>
+  </si>
+  <si>
+    <t>HC6</t>
+  </si>
+  <si>
+    <t>HC7</t>
+  </si>
+  <si>
+    <t>HC8</t>
+  </si>
+  <si>
+    <t>HC9</t>
+  </si>
+  <si>
+    <t>HC10</t>
+  </si>
+  <si>
+    <t>HD1</t>
+  </si>
+  <si>
+    <t>HD2</t>
+  </si>
+  <si>
+    <t>HD3</t>
+  </si>
+  <si>
+    <t>HD4</t>
+  </si>
+  <si>
+    <t>HD5</t>
+  </si>
+  <si>
+    <t>HD6</t>
+  </si>
+  <si>
+    <t>HD7</t>
+  </si>
+  <si>
+    <t>HD8</t>
+  </si>
+  <si>
+    <t>HD9</t>
+  </si>
+  <si>
+    <t>HD10</t>
+  </si>
+  <si>
+    <t>SD1</t>
+  </si>
+  <si>
+    <t>SD2</t>
+  </si>
+  <si>
+    <t>SD3</t>
+  </si>
+  <si>
+    <t>SD4</t>
+  </si>
+  <si>
+    <t>SD5</t>
+  </si>
+  <si>
+    <t>SD6</t>
+  </si>
+  <si>
+    <t>SD7</t>
+  </si>
+  <si>
+    <t>SD8</t>
+  </si>
+  <si>
+    <t>SD9</t>
+  </si>
+  <si>
+    <t>SD10</t>
+  </si>
+  <si>
+    <t>SC1</t>
+  </si>
+  <si>
+    <t>SC2</t>
+  </si>
+  <si>
+    <t>SC3</t>
+  </si>
+  <si>
+    <t>SC4</t>
+  </si>
+  <si>
+    <t>SC5</t>
+  </si>
+  <si>
+    <t>SC6</t>
+  </si>
+  <si>
+    <t>SC7</t>
+  </si>
+  <si>
+    <t>SC8</t>
+  </si>
+  <si>
+    <t>SC9</t>
+  </si>
+  <si>
+    <t>SC10</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>HD</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>Sub-coupled</t>
+  </si>
+  <si>
+    <t>Hyper-divergent</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Sub-divergent</t>
+  </si>
+  <si>
+    <t>Initial family name</t>
+  </si>
+  <si>
+    <t>v.1 famuily code</t>
+  </si>
+  <si>
+    <t>v.1 ID</t>
+  </si>
+  <si>
+    <t>Owner name</t>
+  </si>
+  <si>
+    <t>order in PDF</t>
+  </si>
+  <si>
+    <t>v.2 ID</t>
+  </si>
+  <si>
+    <t>v.2 family code</t>
+  </si>
+  <si>
+    <t>v.2 family name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,8 +673,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -688,6 +863,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -852,7 +1033,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -870,16 +1051,21 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1200,737 +1386,1066 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45:D54"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.9"/>
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="8" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C2" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F4" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F5" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="1" t="s">
+      <c r="G5" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F6" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F7" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="1" t="s">
+      <c r="G7" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="1" t="s">
+      <c r="G8" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="1" t="s">
+      <c r="G9" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F10" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="1" t="s">
+      <c r="G10" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="G11" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C13" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F13" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="1" t="s">
+      <c r="G13" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F14" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="1" t="s">
+      <c r="G14" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F15" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="1" t="s">
+      <c r="G15" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F16" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="1" t="s">
+      <c r="G16" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="1" t="s">
+      <c r="G17" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F18" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="1" t="s">
+      <c r="G18" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="1" t="s">
+      <c r="G19" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F20" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="1" t="s">
+      <c r="G20" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F21" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="1" t="s">
+      <c r="G21" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F22" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="G22" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C24" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F24" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="1" t="s">
+      <c r="G24" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F25" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="1" t="s">
+      <c r="G25" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F26" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="1" t="s">
+      <c r="G26" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F27" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="1" t="s">
+      <c r="G27" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F28" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="1" t="s">
+      <c r="G28" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H28" s="10"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F29" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="1" t="s">
+      <c r="G29" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F30" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="1" t="s">
+      <c r="G30" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F31" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="1" t="s">
+      <c r="G31" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F32" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="1" t="s">
+      <c r="G32" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>27</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F33" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
+      <c r="G33" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C35" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F35" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="1" t="s">
+      <c r="G35" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>31</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F36" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="1" t="s">
+      <c r="G36" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H36" s="10"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F37" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="1" t="s">
+      <c r="G37" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F38" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="1" t="s">
+      <c r="G38" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="H38" s="10"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>34</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F39" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="1" t="s">
+      <c r="G39" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="H39" s="10"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>30</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F40" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="1" t="s">
+      <c r="G40" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="H40" s="10"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F41" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="1" t="s">
+      <c r="G41" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H41" s="10"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="9"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F42" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="1" t="s">
+      <c r="G42" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="H42" s="10"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="9"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E43" t="s">
         <v>36</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F43" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="7"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="1" t="s">
+      <c r="G43" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="H43" s="10"/>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="9"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>37</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F44" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="6"/>
-    </row>
-    <row r="45" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
+      <c r="G44" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H44" s="10"/>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C46" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F46" s="2">
         <v>41</v>
       </c>
-    </row>
-    <row r="46" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="1" t="s">
+      <c r="G46" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F47" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="47" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="7"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="1" t="s">
+      <c r="G47" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H47" s="10"/>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="9"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>43</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F48" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="7"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="1" t="s">
+      <c r="G48" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H48" s="10"/>
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>41</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F49" s="2">
         <v>44</v>
       </c>
-    </row>
-    <row r="49" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="1" t="s">
+      <c r="G49" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="H49" s="10"/>
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>49</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F50" s="2">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="1" t="s">
+      <c r="G50" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="H50" s="10"/>
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="9"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
         <v>47</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F51" s="2">
         <v>46</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="7"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="1" t="s">
+      <c r="G51" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H51" s="10"/>
+      <c r="I51" s="9"/>
+    </row>
+    <row r="52" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="9"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" t="s">
         <v>44</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F52" s="2">
         <v>47</v>
       </c>
-    </row>
-    <row r="52" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="7"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="1" t="s">
+      <c r="G52" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H52" s="10"/>
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="9"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>48</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F53" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="53" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="7"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="1" t="s">
+      <c r="G53" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="H53" s="10"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="9"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E54" t="s">
         <v>42</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F54" s="2">
         <v>49</v>
       </c>
-    </row>
-    <row r="54" spans="2:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="7"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="1" t="s">
+      <c r="G54" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="H54" s="10"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="9"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E55" t="s">
         <v>46</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F55" s="2">
         <v>50</v>
       </c>
+      <c r="G55" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="H55" s="10"/>
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="E45:E54">
-    <sortCondition ref="E45"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E47:E56">
+    <sortCondition ref="E47"/>
   </sortState>
-  <mergeCells count="10">
-    <mergeCell ref="B1:B10"/>
-    <mergeCell ref="B12:B21"/>
-    <mergeCell ref="B23:B32"/>
-    <mergeCell ref="B34:B43"/>
-    <mergeCell ref="B45:B54"/>
-    <mergeCell ref="C1:C10"/>
-    <mergeCell ref="C12:C21"/>
-    <mergeCell ref="C23:C32"/>
-    <mergeCell ref="C34:C43"/>
-    <mergeCell ref="C45:C54"/>
+  <mergeCells count="20">
+    <mergeCell ref="I46:I55"/>
+    <mergeCell ref="I35:I44"/>
+    <mergeCell ref="I24:I33"/>
+    <mergeCell ref="I13:I22"/>
+    <mergeCell ref="I2:I11"/>
+    <mergeCell ref="H2:H11"/>
+    <mergeCell ref="H13:H22"/>
+    <mergeCell ref="H24:H33"/>
+    <mergeCell ref="H35:H44"/>
+    <mergeCell ref="H46:H55"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="C13:C22"/>
+    <mergeCell ref="C24:C33"/>
+    <mergeCell ref="C35:C44"/>
+    <mergeCell ref="C46:C55"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="B13:B22"/>
+    <mergeCell ref="B24:B33"/>
+    <mergeCell ref="B35:B44"/>
+    <mergeCell ref="B46:B55"/>
   </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>